<commit_message>
Nuevos cambios en el documento. Gráficas climáticas
</commit_message>
<xml_diff>
--- a/data/Datos_pobreza_2013.xlsx
+++ b/data/Datos_pobreza_2013.xlsx
@@ -638,7 +638,7 @@
       <name val="@Arial"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +830,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1010,7 +1016,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1042,6 +1048,7 @@
     <xf numFmtId="0" fontId="23" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4049,15 +4056,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -4130,8 +4137,11 @@
       <c r="X1">
         <v>2011</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -4159,8 +4169,11 @@
       <c r="V2">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="X2" s="15">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -4209,8 +4222,11 @@
       <c r="X3">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="15">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4245,7 +4261,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -4285,8 +4301,11 @@
       <c r="X5">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5" s="15">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -4338,8 +4357,11 @@
       <c r="X6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -4374,7 +4396,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -4403,7 +4425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -4420,7 +4442,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -4461,7 +4483,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -4502,7 +4524,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -4522,7 +4544,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -4560,7 +4582,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -4595,7 +4617,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -4627,7 +4649,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -14968,8 +14990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:Y48"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22275,8 +22297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>